<commit_message>
Adds totals to Facility grid
</commit_message>
<xml_diff>
--- a/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.24.1.xlsx
+++ b/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.24.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ShrForms\specifications\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB4B232-FBB4-41F3-BAD1-792C7663A0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B426C81-B0CC-4402-AB6B-4C1A628DA033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2785" uniqueCount="1703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2788" uniqueCount="1706">
   <si>
     <t>Field ID</t>
   </si>
@@ -4993,9 +4993,6 @@
   </si>
   <si>
     <t>LPR103</t>
-  </si>
-  <si>
-    <t>Grid({"page":"facility", "createLabel":"Create Facility", "columns":["LPF004", "LPF001", "LPF009", "LPF010", "LPF011"]})</t>
   </si>
   <si>
     <t>Introduction</t>
@@ -5701,6 +5698,18 @@
   </si>
   <si>
     <t>Return date for current submission must be greater than Return date for previous submission</t>
+  </si>
+  <si>
+    <t>Grid({"page":"facility", "createLabel":"Create Facility", "columns":["LPF004", "LPF001", "LPF009", "LPF010", "LPF011"],totals:["LPF009", "LPF010", "LPF011"]})</t>
+  </si>
+  <si>
+    <t>6.24.1</t>
+  </si>
+  <si>
+    <t>Duncan King</t>
+  </si>
+  <si>
+    <t>Adds totals to Facility grid</t>
   </si>
 </sst>
 </file>
@@ -6888,7 +6897,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6897,7 +6906,7 @@
     <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -6918,19 +6927,19 @@
     <xf numFmtId="0" fontId="32" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8322,9 +8331,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E58"/>
+  <dimension ref="B2:E59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="80" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8941,7 +8952,7 @@
         <v>1004</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
@@ -8955,7 +8966,7 @@
         <v>1004</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
@@ -8969,7 +8980,7 @@
         <v>1004</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
@@ -8977,13 +8988,13 @@
         <v>44322</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>1004</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
@@ -8997,7 +9008,7 @@
         <v>1004</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
@@ -9011,7 +9022,7 @@
         <v>1004</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
@@ -9025,7 +9036,7 @@
         <v>1004</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
@@ -9039,7 +9050,7 @@
         <v>1004</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
@@ -9053,7 +9064,7 @@
         <v>1004</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
@@ -9067,7 +9078,7 @@
         <v>1004</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
@@ -9081,7 +9092,7 @@
         <v>1004</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
@@ -9095,7 +9106,7 @@
         <v>1004</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
@@ -9109,7 +9120,7 @@
         <v>1004</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
@@ -9123,7 +9134,21 @@
         <v>1004</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>1681</v>
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="8">
+        <v>44460</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>1703</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>1704</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>1705</v>
       </c>
     </row>
   </sheetData>
@@ -9597,7 +9622,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="43" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="B34" t="b">
         <f>Data!H147</f>
@@ -10075,7 +10100,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="43" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="B21" t="b">
         <f>Data!H181</f>
@@ -10202,12 +10227,12 @@
       <c r="D8" s="230" t="s">
         <v>173</v>
       </c>
-      <c r="E8" s="233"/>
-      <c r="F8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="232"/>
       <c r="G8" s="230" t="s">
         <v>174</v>
       </c>
-      <c r="H8" s="231"/>
+      <c r="H8" s="232"/>
       <c r="I8" s="73"/>
       <c r="J8" s="73"/>
     </row>
@@ -10215,15 +10240,15 @@
       <c r="C9" s="74">
         <v>1431</v>
       </c>
-      <c r="D9" s="234" t="s">
+      <c r="D9" s="233" t="s">
         <v>446</v>
       </c>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
-      <c r="G9" s="232">
+      <c r="E9" s="233"/>
+      <c r="F9" s="233"/>
+      <c r="G9" s="235">
         <v>1000.1</v>
       </c>
-      <c r="H9" s="232"/>
+      <c r="H9" s="235"/>
       <c r="I9" s="77" t="s">
         <v>1119</v>
       </c>
@@ -10235,15 +10260,15 @@
       <c r="C10" s="74">
         <v>1432</v>
       </c>
-      <c r="D10" s="234" t="s">
+      <c r="D10" s="233" t="s">
         <v>455</v>
       </c>
-      <c r="E10" s="234"/>
-      <c r="F10" s="234"/>
-      <c r="G10" s="232">
+      <c r="E10" s="233"/>
+      <c r="F10" s="233"/>
+      <c r="G10" s="235">
         <v>2000.9</v>
       </c>
-      <c r="H10" s="232"/>
+      <c r="H10" s="235"/>
       <c r="I10" s="77" t="s">
         <v>1119</v>
       </c>
@@ -10268,12 +10293,12 @@
       <c r="D12" s="230" t="s">
         <v>336</v>
       </c>
-      <c r="E12" s="231"/>
+      <c r="E12" s="232"/>
       <c r="F12" s="230" t="s">
         <v>338</v>
       </c>
-      <c r="G12" s="233"/>
-      <c r="H12" s="231"/>
+      <c r="G12" s="231"/>
+      <c r="H12" s="232"/>
       <c r="I12" s="73"/>
       <c r="J12" s="73"/>
     </row>
@@ -10281,15 +10306,15 @@
       <c r="C13" s="74">
         <v>13475</v>
       </c>
-      <c r="D13" s="234" t="s">
+      <c r="D13" s="233" t="s">
         <v>897</v>
       </c>
-      <c r="E13" s="234"/>
-      <c r="F13" s="234" t="s">
+      <c r="E13" s="233"/>
+      <c r="F13" s="233" t="s">
         <v>876</v>
       </c>
-      <c r="G13" s="234"/>
-      <c r="H13" s="234"/>
+      <c r="G13" s="233"/>
+      <c r="H13" s="233"/>
       <c r="I13" s="77" t="s">
         <v>1119</v>
       </c>
@@ -10301,15 +10326,15 @@
       <c r="C14" s="74">
         <v>13476</v>
       </c>
-      <c r="D14" s="234" t="s">
+      <c r="D14" s="233" t="s">
         <v>915</v>
       </c>
-      <c r="E14" s="234"/>
-      <c r="F14" s="234" t="s">
+      <c r="E14" s="233"/>
+      <c r="F14" s="233" t="s">
         <v>878</v>
       </c>
-      <c r="G14" s="234"/>
-      <c r="H14" s="234"/>
+      <c r="G14" s="233"/>
+      <c r="H14" s="233"/>
       <c r="I14" s="77" t="s">
         <v>1119</v>
       </c>
@@ -10519,8 +10544,8 @@
       <c r="E25" s="230" t="s">
         <v>332</v>
       </c>
-      <c r="F25" s="233"/>
-      <c r="G25" s="231"/>
+      <c r="F25" s="231"/>
+      <c r="G25" s="232"/>
       <c r="H25" s="73" t="s">
         <v>1121</v>
       </c>
@@ -10580,12 +10605,12 @@
       <c r="D29" s="230" t="s">
         <v>336</v>
       </c>
-      <c r="E29" s="231"/>
+      <c r="E29" s="232"/>
       <c r="F29" s="230" t="s">
         <v>338</v>
       </c>
-      <c r="G29" s="233"/>
-      <c r="H29" s="231"/>
+      <c r="G29" s="231"/>
+      <c r="H29" s="232"/>
       <c r="I29" s="79"/>
       <c r="J29" s="73"/>
     </row>
@@ -10593,15 +10618,15 @@
       <c r="C30" s="74">
         <v>13473</v>
       </c>
-      <c r="D30" s="234" t="s">
+      <c r="D30" s="233" t="s">
         <v>897</v>
       </c>
-      <c r="E30" s="234"/>
-      <c r="F30" s="234" t="s">
+      <c r="E30" s="233"/>
+      <c r="F30" s="233" t="s">
         <v>876</v>
       </c>
-      <c r="G30" s="234"/>
-      <c r="H30" s="234"/>
+      <c r="G30" s="233"/>
+      <c r="H30" s="233"/>
       <c r="I30" s="77" t="s">
         <v>1119</v>
       </c>
@@ -10613,15 +10638,15 @@
       <c r="C31" s="74">
         <v>13474</v>
       </c>
-      <c r="D31" s="234" t="s">
+      <c r="D31" s="233" t="s">
         <v>919</v>
       </c>
-      <c r="E31" s="234"/>
-      <c r="F31" s="234" t="s">
+      <c r="E31" s="233"/>
+      <c r="F31" s="233" t="s">
         <v>878</v>
       </c>
-      <c r="G31" s="234"/>
-      <c r="H31" s="234"/>
+      <c r="G31" s="233"/>
+      <c r="H31" s="233"/>
       <c r="I31" s="77" t="s">
         <v>1119</v>
       </c>
@@ -10640,11 +10665,11 @@
       <c r="D33" s="230" t="s">
         <v>356</v>
       </c>
-      <c r="E33" s="231"/>
+      <c r="E33" s="232"/>
       <c r="F33" s="230" t="s">
         <v>171</v>
       </c>
-      <c r="G33" s="231"/>
+      <c r="G33" s="232"/>
       <c r="H33" s="80" t="s">
         <v>172</v>
       </c>
@@ -10655,14 +10680,14 @@
       <c r="C34" s="74">
         <v>1454</v>
       </c>
-      <c r="D34" s="234" t="s">
+      <c r="D34" s="233" t="s">
         <v>1138</v>
       </c>
-      <c r="E34" s="234"/>
-      <c r="F34" s="235">
+      <c r="E34" s="233"/>
+      <c r="F34" s="234">
         <v>43133</v>
       </c>
-      <c r="G34" s="235"/>
+      <c r="G34" s="234"/>
       <c r="H34" s="83">
         <v>43134</v>
       </c>
@@ -10677,14 +10702,14 @@
       <c r="C35" s="74">
         <v>1455</v>
       </c>
-      <c r="D35" s="234" t="s">
+      <c r="D35" s="233" t="s">
         <v>1138</v>
       </c>
-      <c r="E35" s="234"/>
-      <c r="F35" s="235">
+      <c r="E35" s="233"/>
+      <c r="F35" s="234">
         <v>43132</v>
       </c>
-      <c r="G35" s="235"/>
+      <c r="G35" s="234"/>
       <c r="H35" s="83">
         <v>43159</v>
       </c>
@@ -10700,6 +10725,24 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="D33:E33"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="F30:H30"/>
@@ -10707,24 +10750,6 @@
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15246,18 +15271,18 @@
     </row>
     <row r="2" spans="1:251" x14ac:dyDescent="0.2">
       <c r="A2" s="87" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B2" s="87"/>
       <c r="C2" s="87" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="D2" s="87"/>
       <c r="E2" s="87" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="3" spans="1:251" x14ac:dyDescent="0.2">
@@ -15278,18 +15303,18 @@
     </row>
     <row r="4" spans="1:251" x14ac:dyDescent="0.2">
       <c r="A4" s="87" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B4" s="87"/>
       <c r="C4" s="87" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="D4" s="87"/>
       <c r="E4" s="87" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="5" spans="1:251" x14ac:dyDescent="0.2">
@@ -15394,14 +15419,14 @@
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="87" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="87" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="F11" s="87" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="12" spans="1:251" x14ac:dyDescent="0.2">
@@ -15410,10 +15435,10 @@
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="32" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="F12" s="38" t="s">
         <v>1015</v>
@@ -16292,8 +16317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA209"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16367,7 +16392,7 @@
       <c r="C4" s="155"/>
       <c r="D4" s="157"/>
       <c r="G4" s="183" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="H4" s="165" t="s">
         <v>437</v>
@@ -16407,7 +16432,7 @@
         <v>44286</v>
       </c>
       <c r="I6" s="165" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="J6" s="165">
         <v>4</v>
@@ -16481,7 +16506,7 @@
         <v>1495</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="W8" s="11" t="s">
         <v>1504</v>
@@ -16544,7 +16569,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="17"/>
       <c r="H10" s="102" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="I10" s="98"/>
       <c r="J10" s="99"/>
@@ -16557,7 +16582,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="O10" s="100"/>
       <c r="P10" s="10"/>
@@ -16593,7 +16618,7 @@
         <v>130</v>
       </c>
       <c r="F11" s="106" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G11" s="107"/>
       <c r="H11" s="101">
@@ -16601,7 +16626,7 @@
       </c>
       <c r="I11" s="105"/>
       <c r="J11" s="99" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="K11" s="106" t="s">
         <v>131</v>
@@ -16642,7 +16667,7 @@
         <v>1258</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="103">
@@ -16661,7 +16686,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="99" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="O12" s="100"/>
       <c r="P12" s="10"/>
@@ -16690,13 +16715,13 @@
         <v>Submission.LPR005</v>
       </c>
       <c r="D13" s="107" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="E13" s="106" t="s">
         <v>128</v>
       </c>
       <c r="F13" s="106" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G13" s="107"/>
       <c r="H13" s="104">
@@ -16740,7 +16765,7 @@
         <v>Submission.LPR005a</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>128</v>
@@ -16752,7 +16777,7 @@
       </c>
       <c r="I14" s="104"/>
       <c r="J14" s="99" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>129</v>
@@ -16765,14 +16790,14 @@
         <v>1</v>
       </c>
       <c r="N14" s="16" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="O14" s="100" t="b">
         <f>H14&lt;=H196</f>
         <v>1</v>
       </c>
       <c r="P14" s="16" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="Q14" s="100"/>
       <c r="R14" s="10"/>
@@ -16802,7 +16827,7 @@
         <v>1166</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="17"/>
@@ -17054,7 +17079,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="O20" s="100"/>
       <c r="P20" s="10"/>
@@ -17131,7 +17156,7 @@
         <v>1006</v>
       </c>
       <c r="E22" s="176" t="s">
-        <v>1525</v>
+        <v>1702</v>
       </c>
       <c r="F22" s="177"/>
       <c r="G22" s="178"/>
@@ -17160,17 +17185,17 @@
     <row r="23" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15"/>
       <c r="B23" s="174" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C23" s="181" t="str">
         <f>"Submission." &amp; B23</f>
         <v>Submission.LPR104</v>
       </c>
       <c r="D23" s="175" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="E23" s="176" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="F23" s="177"/>
       <c r="G23" s="178"/>
@@ -17209,7 +17234,7 @@
         <v>1520</v>
       </c>
       <c r="E24" s="176" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="F24" s="177"/>
       <c r="G24" s="178"/>
@@ -17248,7 +17273,7 @@
         <v>1519</v>
       </c>
       <c r="E25" s="176" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="F25" s="177"/>
       <c r="G25" s="178"/>
@@ -17344,7 +17369,7 @@
     </row>
     <row r="28" spans="1:26" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="23" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="C28" s="116" t="str">
         <f t="shared" ref="C28:C55" si="2">"IGFLend." &amp; B28</f>
@@ -17564,7 +17589,7 @@
         <v>1</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="O32" s="100"/>
       <c r="P32" s="10"/>
@@ -17642,7 +17667,7 @@
         <v>188</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="17"/>
@@ -17787,7 +17812,7 @@
         <v>IGFLend.LPIGF009</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>128</v>
@@ -17833,7 +17858,7 @@
         <v>IGFLend.LPIGF010</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>128</v>
@@ -17977,7 +18002,7 @@
         <v>193</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="17"/>
@@ -18175,7 +18200,7 @@
         <v>1273</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="17"/>
@@ -18276,7 +18301,7 @@
         <v>1275</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="17"/>
@@ -18325,7 +18350,7 @@
         <v>1276</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="17"/>
@@ -18463,7 +18488,7 @@
         <v>IGFLend.LPC020bx</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>387</v>
@@ -18564,7 +18589,7 @@
         <v>1279</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="17"/>
@@ -18662,7 +18687,7 @@
         <v>1281</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="17"/>
@@ -18690,7 +18715,7 @@
         <v>0</v>
       </c>
       <c r="X55" s="10" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="Y55" s="29" t="s">
         <v>230</v>
@@ -18949,7 +18974,7 @@
         <v>1</v>
       </c>
       <c r="N61" s="10" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="O61" s="100"/>
       <c r="P61" s="10"/>
@@ -19172,7 +19197,7 @@
         <v>IGFBorrow.LPIGF033</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="E66" s="9" t="s">
         <v>128</v>
@@ -19218,7 +19243,7 @@
         <v>IGFBorrow.LPIGF034</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>128</v>
@@ -19850,7 +19875,7 @@
         <v>IGFBorrow.LPIGF044x</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>387</v>
@@ -19905,7 +19930,7 @@
         <v>1426</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="F81" s="9"/>
       <c r="G81" s="17"/>
@@ -19933,7 +19958,7 @@
         <v>0</v>
       </c>
       <c r="X81" s="16" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="Y81" s="26" t="s">
         <v>250</v>
@@ -20001,7 +20026,7 @@
         <v>1</v>
       </c>
       <c r="N83" s="10" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="O83" s="100"/>
       <c r="P83" s="10"/>
@@ -20080,7 +20105,7 @@
         <v>173</v>
       </c>
       <c r="E85" s="23" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="F85" s="9"/>
       <c r="G85" s="17"/>
@@ -20146,7 +20171,7 @@
         <v>1</v>
       </c>
       <c r="N86" s="10" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="O86" s="100"/>
       <c r="P86" s="10"/>
@@ -20272,7 +20297,7 @@
         <v>176</v>
       </c>
       <c r="E89" s="23" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="F89" s="9"/>
       <c r="G89" s="17"/>
@@ -20355,7 +20380,7 @@
     </row>
     <row r="91" spans="1:26" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="23" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C91" s="116" t="str">
         <f t="shared" si="4"/>
@@ -20409,7 +20434,7 @@
         <v>ISDA.LPC025b</v>
       </c>
       <c r="D92" s="16" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>387</v>
@@ -20695,7 +20720,7 @@
         <v>182</v>
       </c>
       <c r="E98" s="23" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="F98" s="9"/>
       <c r="G98" s="17"/>
@@ -20742,7 +20767,7 @@
         <v>183</v>
       </c>
       <c r="E99" s="23" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="F99" s="9"/>
       <c r="G99" s="17"/>
@@ -20779,7 +20804,7 @@
     <row r="100" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="15"/>
       <c r="B100" s="174" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C100" s="181" t="str">
         <f>"ISDA." &amp; B100</f>
@@ -20789,7 +20814,7 @@
         <v>1005</v>
       </c>
       <c r="E100" s="177" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="F100" s="177"/>
       <c r="G100" s="178"/>
@@ -20951,7 +20976,7 @@
         <v>336</v>
       </c>
       <c r="E104" s="23" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="F104" s="9"/>
       <c r="G104" s="17"/>
@@ -20988,7 +21013,7 @@
         <v>64</v>
       </c>
       <c r="B105" s="23" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C105" s="116" t="str">
         <f t="shared" si="5"/>
@@ -21038,7 +21063,7 @@
         <v>65</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="C106" s="116" t="str">
         <f t="shared" si="5"/>
@@ -21085,7 +21110,7 @@
         <v>66</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="C107" s="116" t="str">
         <f t="shared" si="5"/>
@@ -21132,7 +21157,7 @@
         <v>67</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="C108" s="116" t="str">
         <f t="shared" si="5"/>
@@ -21179,7 +21204,7 @@
         <v>68</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="C109" s="116" t="str">
         <f t="shared" si="5"/>
@@ -21308,7 +21333,7 @@
         <v>Facility.LPF001</v>
       </c>
       <c r="D112" s="16" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="E112" s="23" t="s">
         <v>1331</v>
@@ -21320,7 +21345,7 @@
       </c>
       <c r="I112" s="103"/>
       <c r="J112" s="102" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="K112" s="9" t="s">
         <v>129</v>
@@ -21395,7 +21420,7 @@
     </row>
     <row r="114" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B114" s="23" t="s">
         <v>21</v>
@@ -21408,7 +21433,7 @@
         <v>342</v>
       </c>
       <c r="E114" s="23" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="F114" s="9"/>
       <c r="G114" s="17"/>
@@ -21465,7 +21490,7 @@
       </c>
       <c r="F115" s="106"/>
       <c r="G115" s="107" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="H115" s="101"/>
       <c r="I115" s="199" t="str">
@@ -21473,7 +21498,7 @@
         <v>DMOBOS002</v>
       </c>
       <c r="J115" s="117" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="K115" s="106"/>
       <c r="L115" s="107"/>
@@ -21554,7 +21579,7 @@
         <v>1344</v>
       </c>
       <c r="E117" s="23" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="F117" s="9"/>
       <c r="G117" s="17"/>
@@ -21828,14 +21853,14 @@
         <v>1</v>
       </c>
       <c r="N122" s="10" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="O122" s="100" t="b">
         <f>H122=pfo_total_loan_lpl007</f>
         <v>1</v>
       </c>
       <c r="P122" s="93" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="Q122" s="100"/>
       <c r="R122" s="10"/>
@@ -21960,7 +21985,7 @@
         <v>402</v>
       </c>
       <c r="E125" s="23" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="F125" s="9"/>
       <c r="G125" s="17"/>
@@ -22286,7 +22311,7 @@
         <v>1359</v>
       </c>
       <c r="E132" s="175" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="F132" s="9"/>
       <c r="G132" s="17"/>
@@ -22314,7 +22339,7 @@
         <v>0</v>
       </c>
       <c r="X132" s="10" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="Y132" s="16" t="s">
         <v>259</v>
@@ -22336,7 +22361,7 @@
         <v>1040</v>
       </c>
       <c r="E133" s="176" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="F133" s="177"/>
       <c r="G133" s="178"/>
@@ -22452,7 +22477,7 @@
         <v>162</v>
       </c>
       <c r="E136" s="23" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="F136" s="9"/>
       <c r="G136" s="17"/>
@@ -22479,7 +22504,7 @@
         <v>0</v>
       </c>
       <c r="P136" s="10" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="Q136" s="100"/>
       <c r="R136" s="10"/>
@@ -22519,7 +22544,7 @@
         <v>BOSVAR002</v>
       </c>
       <c r="J137" s="117" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="K137" s="106"/>
       <c r="L137" s="107"/>
@@ -22555,7 +22580,7 @@
         <v>163</v>
       </c>
       <c r="E138" s="23" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="F138" s="9"/>
       <c r="G138" s="17"/>
@@ -22818,7 +22843,7 @@
         <v>166</v>
       </c>
       <c r="E143" s="23" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="F143" s="9"/>
       <c r="G143" s="17"/>
@@ -22861,7 +22886,7 @@
         <v>167</v>
       </c>
       <c r="E144" s="23" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="F144" s="9"/>
       <c r="G144" s="17"/>
@@ -22870,7 +22895,7 @@
       </c>
       <c r="I144" s="103"/>
       <c r="J144" s="99" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="K144" s="9" t="s">
         <v>129</v>
@@ -22947,7 +22972,7 @@
         <v>1</v>
       </c>
       <c r="N145" s="10" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="O145" s="100"/>
       <c r="P145" s="10"/>
@@ -22969,7 +22994,7 @@
     </row>
     <row r="146" spans="2:27" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="23" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C146" s="116" t="str">
         <f t="shared" si="7"/>
@@ -22997,7 +23022,7 @@
         <v>0</v>
       </c>
       <c r="N146" s="10" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="O146" s="100"/>
       <c r="P146" s="10"/>
@@ -23026,7 +23051,7 @@
         <v>Loan.LPL010b</v>
       </c>
       <c r="D147" s="16" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="E147" s="23" t="s">
         <v>387</v>
@@ -23210,21 +23235,21 @@
         <v>1</v>
       </c>
       <c r="N150" s="10" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="O150" s="100" t="b">
         <f>IF(OR(H143=4,H143=5,H143=10),H150&lt;H149, TRUE)</f>
         <v>1</v>
       </c>
       <c r="P150" s="10" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="Q150" s="100" t="b">
         <f>IF(OR(H143=9,H143=11),H150&lt;H148, TRUE)</f>
         <v>1</v>
       </c>
       <c r="R150" s="10" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="S150" s="100" t="b">
         <f>H150&gt;=H119</f>
@@ -23238,7 +23263,7 @@
         <v>1</v>
       </c>
       <c r="V150" s="10" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="W150" s="116" t="b">
         <f>AND( H144&lt;&gt;4,H144&lt;&gt;5)</f>
@@ -23416,7 +23441,7 @@
         <v>966</v>
       </c>
       <c r="E154" s="23" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="F154" s="9"/>
       <c r="G154" s="17"/>
@@ -23436,7 +23461,7 @@
         <v>0</v>
       </c>
       <c r="N154" s="10" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="O154" s="100"/>
       <c r="P154" s="10"/>
@@ -23819,7 +23844,7 @@
         <v>1</v>
       </c>
       <c r="P162" s="10" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="Q162" s="100"/>
       <c r="R162" s="10"/>
@@ -23851,7 +23876,7 @@
         <v>998</v>
       </c>
       <c r="E163" s="175" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="F163" s="9"/>
       <c r="G163" s="17"/>
@@ -23879,7 +23904,7 @@
         <v>0</v>
       </c>
       <c r="X163" s="10" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="Y163" s="16" t="s">
         <v>302</v>
@@ -23891,17 +23916,17 @@
     <row r="164" spans="1:27" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="15"/>
       <c r="B164" s="174" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="C164" s="116" t="str">
         <f>"Loan." &amp; B164</f>
         <v>Loan.LPL101</v>
       </c>
       <c r="D164" s="175" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="E164" s="176" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="F164" s="177"/>
       <c r="G164" s="178"/>
@@ -23930,17 +23955,17 @@
     <row r="165" spans="1:27" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="15"/>
       <c r="B165" s="174" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="C165" s="116" t="str">
         <f t="shared" si="7"/>
         <v>Loan.LPL100</v>
       </c>
       <c r="D165" s="175" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="E165" s="176" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="F165" s="177"/>
       <c r="G165" s="178"/>
@@ -24374,7 +24399,7 @@
         <v>1481</v>
       </c>
       <c r="E175" s="23" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="F175" s="9"/>
       <c r="G175" s="17"/>
@@ -24437,7 +24462,7 @@
         <v>1</v>
       </c>
       <c r="N176" s="10" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="O176" s="100"/>
       <c r="P176" s="10"/>
@@ -24530,7 +24555,7 @@
         <v>1</v>
       </c>
       <c r="N178" s="10" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="O178" s="100"/>
       <c r="P178" s="10"/>
@@ -24641,14 +24666,14 @@
     </row>
     <row r="181" spans="1:26" s="18" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="23" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="C181" s="116" t="str">
         <f t="shared" si="9"/>
         <v>EIRD.LPC018c</v>
       </c>
       <c r="D181" s="16" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="E181" s="23" t="s">
         <v>387</v>
@@ -24669,7 +24694,7 @@
         <v>1</v>
       </c>
       <c r="N181" s="10" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="O181" s="100"/>
       <c r="P181" s="10"/>
@@ -24726,7 +24751,7 @@
         <v>1373</v>
       </c>
       <c r="D183" s="123" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="E183" s="23" t="s">
         <v>128</v>
@@ -24854,16 +24879,16 @@
     </row>
     <row r="186" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B186" s="23" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="C186" s="62" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D186" s="123" t="s">
         <v>1530</v>
       </c>
-      <c r="D186" s="123" t="s">
+      <c r="E186" s="23" t="s">
         <v>1531</v>
-      </c>
-      <c r="E186" s="23" t="s">
-        <v>1532</v>
       </c>
       <c r="F186" s="23"/>
       <c r="G186" s="23"/>
@@ -24916,7 +24941,7 @@
     </row>
     <row r="188" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B188" s="126" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C188" s="127" t="s">
         <v>1381</v>
@@ -24928,7 +24953,7 @@
         <v>1383</v>
       </c>
       <c r="F188" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G188" s="127"/>
       <c r="H188" s="99" t="s">
@@ -24955,7 +24980,7 @@
     </row>
     <row r="189" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B189" s="126" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C189" s="127" t="s">
         <v>1385</v>
@@ -24971,7 +24996,7 @@
       </c>
       <c r="G189" s="127"/>
       <c r="H189" s="99" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="I189" s="99"/>
       <c r="J189" s="99"/>
@@ -24994,7 +25019,7 @@
     </row>
     <row r="190" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B190" s="126" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C190" s="127" t="s">
         <v>1388</v>
@@ -25006,11 +25031,11 @@
         <v>1387</v>
       </c>
       <c r="F190" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G190" s="127"/>
       <c r="H190" s="99" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="I190" s="99"/>
       <c r="J190" s="99"/>
@@ -25033,7 +25058,7 @@
     </row>
     <row r="191" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B191" s="126" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C191" s="127" t="s">
         <v>1389</v>
@@ -25045,7 +25070,7 @@
         <v>1391</v>
       </c>
       <c r="F191" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G191" s="127"/>
       <c r="H191" s="118">
@@ -25072,7 +25097,7 @@
     </row>
     <row r="192" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B192" s="126" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="C192" s="127" t="s">
         <v>1392</v>
@@ -25084,7 +25109,7 @@
         <v>1391</v>
       </c>
       <c r="F192" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G192" s="127"/>
       <c r="H192" s="118">
@@ -25111,7 +25136,7 @@
     </row>
     <row r="193" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B193" s="126" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C193" s="127" t="s">
         <v>1394</v>
@@ -25123,7 +25148,7 @@
         <v>1396</v>
       </c>
       <c r="F193" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G193" s="127"/>
       <c r="H193" s="99" t="s">
@@ -25150,16 +25175,16 @@
     </row>
     <row r="194" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B194" s="126" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="C194" s="127" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="D194" s="127" t="s">
+        <v>1580</v>
+      </c>
+      <c r="E194" s="126" t="s">
         <v>1581</v>
-      </c>
-      <c r="E194" s="126" t="s">
-        <v>1582</v>
       </c>
       <c r="F194" s="126" t="s">
         <v>1256</v>
@@ -25189,13 +25214,13 @@
     </row>
     <row r="195" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B195" s="126" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="C195" s="127" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="D195" s="127" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="E195" s="126" t="s">
         <v>1400</v>
@@ -25228,22 +25253,22 @@
     </row>
     <row r="196" spans="1:26" s="208" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="126" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B196" s="126" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C196" s="127" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D196" s="127" t="s">
+        <v>1700</v>
+      </c>
+      <c r="E196" s="126" t="s">
         <v>1686</v>
       </c>
-      <c r="B196" s="126" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C196" s="127" t="s">
-        <v>1688</v>
-      </c>
-      <c r="D196" s="127" t="s">
-        <v>1701</v>
-      </c>
-      <c r="E196" s="126" t="s">
-        <v>1687</v>
-      </c>
       <c r="F196" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G196" s="126"/>
       <c r="H196" s="118">
@@ -25272,7 +25297,7 @@
     </row>
     <row r="197" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B197" s="126" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="C197" s="127" t="s">
         <v>1398</v>
@@ -25284,7 +25309,7 @@
         <v>1400</v>
       </c>
       <c r="F197" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G197" s="127"/>
       <c r="H197" s="97">
@@ -25311,7 +25336,7 @@
     </row>
     <row r="198" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B198" s="126" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="C198" s="127" t="s">
         <v>1401</v>
@@ -25323,7 +25348,7 @@
         <v>1400</v>
       </c>
       <c r="F198" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G198" s="127"/>
       <c r="H198" s="97">
@@ -25350,7 +25375,7 @@
     </row>
     <row r="199" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B199" s="126" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="C199" s="127" t="s">
         <v>1403</v>
@@ -25362,7 +25387,7 @@
         <v>1400</v>
       </c>
       <c r="F199" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G199" s="127"/>
       <c r="H199" s="97">
@@ -25389,7 +25414,7 @@
     </row>
     <row r="200" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B200" s="126" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="C200" s="127" t="s">
         <v>1405</v>
@@ -25401,7 +25426,7 @@
         <v>1439</v>
       </c>
       <c r="F200" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G200" s="127"/>
       <c r="H200" s="97">
@@ -25428,7 +25453,7 @@
     </row>
     <row r="201" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B201" s="126" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C201" s="127" t="s">
         <v>1407</v>
@@ -25440,7 +25465,7 @@
         <v>1400</v>
       </c>
       <c r="F201" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G201" s="127"/>
       <c r="H201" s="97">
@@ -25468,7 +25493,7 @@
     </row>
     <row r="202" spans="1:26" ht="318.75" x14ac:dyDescent="0.2">
       <c r="B202" s="126" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C202" s="127" t="s">
         <v>1409</v>
@@ -25482,7 +25507,7 @@
       <c r="F202" s="126"/>
       <c r="G202" s="127"/>
       <c r="H202" s="118" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="I202" s="118"/>
       <c r="J202" s="99"/>
@@ -25503,7 +25528,7 @@
     </row>
     <row r="203" spans="1:26" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B203" s="126" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="C203" s="127" t="s">
         <v>1412</v>
@@ -25517,7 +25542,7 @@
       <c r="F203" s="126"/>
       <c r="G203" s="127"/>
       <c r="H203" s="118" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="I203" s="118"/>
       <c r="J203" s="99"/>
@@ -25538,7 +25563,7 @@
     </row>
     <row r="204" spans="1:26" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B204" s="126" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="C204" s="127" t="s">
         <v>1414</v>
@@ -25552,7 +25577,7 @@
       <c r="F204" s="126"/>
       <c r="G204" s="127"/>
       <c r="H204" s="118" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="I204" s="118"/>
       <c r="J204" s="99"/>
@@ -25573,7 +25598,7 @@
     </row>
     <row r="205" spans="1:26" ht="229.5" x14ac:dyDescent="0.2">
       <c r="B205" s="126" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="C205" s="127" t="s">
         <v>1416</v>
@@ -25608,23 +25633,23 @@
     </row>
     <row r="206" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B206" s="162" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C206" s="184" t="s">
+        <v>1548</v>
+      </c>
+      <c r="D206" s="184" t="s">
         <v>1549</v>
-      </c>
-      <c r="D206" s="184" t="s">
-        <v>1550</v>
       </c>
       <c r="E206" s="126" t="s">
         <v>1387</v>
       </c>
       <c r="F206" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G206" s="184"/>
       <c r="H206" s="185" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="I206" s="185"/>
       <c r="J206" s="185"/>
@@ -25647,19 +25672,19 @@
     </row>
     <row r="207" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B207" s="162" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C207" s="184" t="s">
         <v>1568</v>
       </c>
-      <c r="C207" s="184" t="s">
+      <c r="D207" s="184" t="s">
         <v>1569</v>
-      </c>
-      <c r="D207" s="184" t="s">
-        <v>1570</v>
       </c>
       <c r="E207" s="161" t="s">
         <v>1391</v>
       </c>
       <c r="F207" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G207" s="184"/>
       <c r="H207" s="188">
@@ -25686,19 +25711,19 @@
     </row>
     <row r="208" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B208" s="162" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C208" s="184" t="s">
+        <v>1570</v>
+      </c>
+      <c r="D208" s="184" t="s">
         <v>1571</v>
-      </c>
-      <c r="D208" s="184" t="s">
-        <v>1572</v>
       </c>
       <c r="E208" s="161" t="s">
         <v>1391</v>
       </c>
       <c r="F208" s="126" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G208" s="184"/>
       <c r="H208" s="188">
@@ -25856,7 +25881,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="43" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="B14" t="str">
         <f>Data!H16</f>
@@ -25865,7 +25890,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="43" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B16">
         <f>Data!H17</f>
@@ -25874,7 +25899,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B18">
         <f>Data!H18</f>
@@ -25883,7 +25908,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="43" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B20" s="137">
         <f>Data!I19</f>
@@ -25892,7 +25917,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="43" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="B22" s="111">
         <f>Data!H20</f>
@@ -25901,7 +25926,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="43" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="B24">
         <f>Data!H21</f>
@@ -26216,7 +26241,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="B10" s="110">
         <f>Data!H14</f>
@@ -26228,7 +26253,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="43" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="B12" t="str">
         <f>Data!H15</f>
@@ -26237,7 +26262,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="43" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="B14" t="str">
         <f>Data!H16</f>
@@ -26246,7 +26271,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="43" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B16">
         <f>Data!H17</f>
@@ -26255,7 +26280,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B18">
         <f>Data!H18</f>
@@ -26264,7 +26289,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="43" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B20" s="137">
         <f>Data!I19</f>
@@ -26273,7 +26298,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="43" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="B22" s="111">
         <f>Data!H20</f>
@@ -26282,7 +26307,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="43" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="B24">
         <f>Data!H21</f>
@@ -26303,7 +26328,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" s="32" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -26315,7 +26340,7 @@
         <v>1343</v>
       </c>
       <c r="C31" s="215" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="D31" s="216"/>
       <c r="E31" s="79" t="s">
@@ -26328,7 +26353,7 @@
         <v>159</v>
       </c>
       <c r="H31" s="79" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="I31" s="207" t="s">
         <v>1121</v>
@@ -26340,11 +26365,11 @@
         <f>Data!I115</f>
         <v>DMOBOS002</v>
       </c>
-      <c r="C32" s="224" t="str">
+      <c r="C32" s="221" t="str">
         <f>Data!H112</f>
         <v>BOS</v>
       </c>
-      <c r="D32" s="224"/>
+      <c r="D32" s="221"/>
       <c r="E32" s="138">
         <f>Data!H121</f>
         <v>20000</v>
@@ -26358,10 +26383,10 @@
         <v>0</v>
       </c>
       <c r="H32" s="209" t="s">
+        <v>1690</v>
+      </c>
+      <c r="I32" s="209" t="s">
         <v>1691</v>
-      </c>
-      <c r="I32" s="209" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -26388,13 +26413,13 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="43"/>
       <c r="B35" s="43" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="43"/>
       <c r="B36" s="32" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -26417,10 +26442,10 @@
         <v>340</v>
       </c>
       <c r="G38" s="79" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="H38" s="79" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="I38" s="207" t="s">
         <v>1121</v>
@@ -26432,11 +26457,11 @@
         <f>Data!H167</f>
         <v>Debt Service Test (DST)</v>
       </c>
-      <c r="C39" s="221" t="str">
+      <c r="C39" s="224" t="str">
         <f>Data!H168</f>
         <v>This is how the Covenant is calculated…</v>
       </c>
-      <c r="D39" s="221"/>
+      <c r="D39" s="224"/>
       <c r="E39" s="210" t="str">
         <f>Data!H169</f>
         <v>105%</v>
@@ -26450,10 +26475,10 @@
         <v>40269</v>
       </c>
       <c r="H39" s="209" t="s">
+        <v>1690</v>
+      </c>
+      <c r="I39" s="209" t="s">
         <v>1691</v>
-      </c>
-      <c r="I39" s="209" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -26468,7 +26493,7 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="43"/>
       <c r="B42" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -26486,13 +26511,13 @@
       </c>
       <c r="E44" s="223"/>
       <c r="F44" s="79" t="s">
+        <v>1533</v>
+      </c>
+      <c r="G44" s="79" t="s">
         <v>1534</v>
       </c>
-      <c r="G44" s="79" t="s">
-        <v>1535</v>
-      </c>
       <c r="H44" s="79" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="I44" s="207" t="s">
         <v>1121</v>
@@ -26519,10 +26544,10 @@
         <v>55153</v>
       </c>
       <c r="H45" s="209" t="s">
+        <v>1690</v>
+      </c>
+      <c r="I45" s="209" t="s">
         <v>1691</v>
-      </c>
-      <c r="I45" s="209" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -26537,7 +26562,7 @@
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="43"/>
       <c r="B48" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -26555,13 +26580,13 @@
       </c>
       <c r="E50" s="223"/>
       <c r="F50" s="79" t="s">
+        <v>1533</v>
+      </c>
+      <c r="G50" s="79" t="s">
         <v>1534</v>
       </c>
-      <c r="G50" s="79" t="s">
-        <v>1535</v>
-      </c>
       <c r="H50" s="79" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="I50" s="207" t="s">
         <v>1121</v>
@@ -26588,10 +26613,10 @@
         <v>49399</v>
       </c>
       <c r="H51" s="209" t="s">
+        <v>1690</v>
+      </c>
+      <c r="I51" s="209" t="s">
         <v>1691</v>
-      </c>
-      <c r="I51" s="209" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
@@ -26609,7 +26634,7 @@
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="43"/>
       <c r="B54" s="32" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -26631,7 +26656,7 @@
       </c>
       <c r="G56" s="216"/>
       <c r="H56" s="79" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="I56" s="207" t="s">
         <v>1121</v>
@@ -26655,10 +26680,10 @@
       </c>
       <c r="G57" s="220"/>
       <c r="H57" s="209" t="s">
+        <v>1690</v>
+      </c>
+      <c r="I57" s="209" t="s">
         <v>1691</v>
-      </c>
-      <c r="I57" s="209" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
@@ -26667,11 +26692,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C38:D38"/>
     <mergeCell ref="C57:E57"/>
     <mergeCell ref="F57:G57"/>
     <mergeCell ref="F56:G56"/>
@@ -26686,6 +26706,11 @@
     <mergeCell ref="D50:E50"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="D51:E51"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26941,7 +26966,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="43" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="B56" t="b">
         <f>Data!H51</f>
@@ -27239,7 +27264,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="43" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="B56" t="b">
         <f>Data!H80</f>
@@ -27363,7 +27388,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="B26" t="b">
         <f>Data!H92</f>

</xml_diff>